<commit_message>
GK: backround files fix pumas update du to in_jeru add
</commit_message>
<xml_diff>
--- a/create_forecast_basic/arab_and_palestinian/Intermediates/taz_Arab_Palestinian_2025.xlsx
+++ b/create_forecast_basic/arab_and_palestinian/Intermediates/taz_Arab_Palestinian_2025.xlsx
@@ -5361,7 +5361,7 @@
       </c>
       <c r="B93" t="inlineStr"/>
       <c r="C93" t="n">
-        <v>1151.44999641891</v>
+        <v>1151.449996418909</v>
       </c>
       <c r="D93" t="inlineStr"/>
       <c r="E93" t="inlineStr"/>
@@ -5386,7 +5386,7 @@
       </c>
       <c r="B94" t="inlineStr"/>
       <c r="C94" t="n">
-        <v>3585.602196402347</v>
+        <v>3585.602196402348</v>
       </c>
       <c r="D94" t="inlineStr"/>
       <c r="E94" t="inlineStr"/>
@@ -5411,7 +5411,7 @@
       </c>
       <c r="B95" t="inlineStr"/>
       <c r="C95" t="n">
-        <v>3170.239689626988</v>
+        <v>3170.239689626991</v>
       </c>
       <c r="D95" t="inlineStr"/>
       <c r="E95" t="inlineStr"/>
@@ -5436,7 +5436,7 @@
       </c>
       <c r="B96" t="inlineStr"/>
       <c r="C96" t="n">
-        <v>14613.08903873925</v>
+        <v>14613.08903873924</v>
       </c>
       <c r="D96" t="inlineStr"/>
       <c r="E96" t="inlineStr"/>
@@ -5486,7 +5486,7 @@
       </c>
       <c r="B98" t="inlineStr"/>
       <c r="C98" t="n">
-        <v>8287.759301245358</v>
+        <v>8287.759301245351</v>
       </c>
       <c r="D98" t="inlineStr"/>
       <c r="E98" t="inlineStr"/>
@@ -5561,7 +5561,7 @@
       </c>
       <c r="B101" t="inlineStr"/>
       <c r="C101" t="n">
-        <v>14112.74184024463</v>
+        <v>14112.74184024464</v>
       </c>
       <c r="D101" t="inlineStr"/>
       <c r="E101" t="inlineStr"/>
@@ -5586,7 +5586,7 @@
       </c>
       <c r="B102" t="inlineStr"/>
       <c r="C102" t="n">
-        <v>9104.686041597433</v>
+        <v>9104.686041597432</v>
       </c>
       <c r="D102" t="inlineStr"/>
       <c r="E102" t="inlineStr"/>
@@ -5611,7 +5611,7 @@
       </c>
       <c r="B103" t="inlineStr"/>
       <c r="C103" t="n">
-        <v>35003.65250121392</v>
+        <v>35003.65250121394</v>
       </c>
       <c r="D103" t="inlineStr"/>
       <c r="E103" t="inlineStr"/>
@@ -5661,7 +5661,7 @@
       </c>
       <c r="B105" t="inlineStr"/>
       <c r="C105" t="n">
-        <v>25876.76852095268</v>
+        <v>25876.76852095266</v>
       </c>
       <c r="D105" t="inlineStr"/>
       <c r="E105" t="inlineStr"/>
@@ -5686,7 +5686,7 @@
       </c>
       <c r="B106" t="inlineStr"/>
       <c r="C106" t="n">
-        <v>9885.020915381157</v>
+        <v>9885.020915381163</v>
       </c>
       <c r="D106" t="inlineStr"/>
       <c r="E106" t="inlineStr"/>
@@ -5711,7 +5711,7 @@
       </c>
       <c r="B107" t="inlineStr"/>
       <c r="C107" t="n">
-        <v>1451.83944746431</v>
+        <v>1451.839447464311</v>
       </c>
       <c r="D107" t="inlineStr"/>
       <c r="E107" t="inlineStr"/>
@@ -5736,7 +5736,7 @@
       </c>
       <c r="B108" t="inlineStr"/>
       <c r="C108" t="n">
-        <v>7113.190258109426</v>
+        <v>7113.190258109428</v>
       </c>
       <c r="D108" t="inlineStr"/>
       <c r="E108" t="inlineStr"/>
@@ -5786,7 +5786,7 @@
       </c>
       <c r="B110" t="inlineStr"/>
       <c r="C110" t="n">
-        <v>2244.180795983397</v>
+        <v>2244.180795983398</v>
       </c>
       <c r="D110" t="inlineStr"/>
       <c r="E110" t="inlineStr"/>
@@ -5811,7 +5811,7 @@
       </c>
       <c r="B111" t="inlineStr"/>
       <c r="C111" t="n">
-        <v>12823.05247958681</v>
+        <v>12823.0524795868</v>
       </c>
       <c r="D111" t="inlineStr"/>
       <c r="E111" t="inlineStr"/>
@@ -5861,7 +5861,7 @@
       </c>
       <c r="B113" t="inlineStr"/>
       <c r="C113" t="n">
-        <v>9907.900963974977</v>
+        <v>9907.900963974978</v>
       </c>
       <c r="D113" t="inlineStr"/>
       <c r="E113" t="inlineStr"/>
@@ -5936,7 +5936,7 @@
       </c>
       <c r="B116" t="inlineStr"/>
       <c r="C116" t="n">
-        <v>3024.107919695308</v>
+        <v>3024.107919695306</v>
       </c>
       <c r="D116" t="inlineStr"/>
       <c r="E116" t="inlineStr"/>
@@ -5961,7 +5961,7 @@
       </c>
       <c r="B117" t="inlineStr"/>
       <c r="C117" t="n">
-        <v>7509.71584924435</v>
+        <v>7509.715849244338</v>
       </c>
       <c r="D117" t="inlineStr"/>
       <c r="E117" t="inlineStr"/>
@@ -6011,7 +6011,7 @@
       </c>
       <c r="B119" t="inlineStr"/>
       <c r="C119" t="n">
-        <v>6927.790978093692</v>
+        <v>6927.790978093689</v>
       </c>
       <c r="D119" t="inlineStr"/>
       <c r="E119" t="inlineStr"/>
@@ -6111,7 +6111,7 @@
       </c>
       <c r="B123" t="inlineStr"/>
       <c r="C123" t="n">
-        <v>33953.28146071259</v>
+        <v>33953.28146071261</v>
       </c>
       <c r="D123" t="inlineStr"/>
       <c r="E123" t="inlineStr"/>
@@ -6136,7 +6136,7 @@
       </c>
       <c r="B124" t="inlineStr"/>
       <c r="C124" t="n">
-        <v>9072.841744888967</v>
+        <v>9072.841744888972</v>
       </c>
       <c r="D124" t="inlineStr"/>
       <c r="E124" t="inlineStr"/>
@@ -6161,7 +6161,7 @@
       </c>
       <c r="B125" t="inlineStr"/>
       <c r="C125" t="n">
-        <v>11465.33216020146</v>
+        <v>11465.33216020145</v>
       </c>
       <c r="D125" t="inlineStr"/>
       <c r="E125" t="inlineStr"/>
@@ -6186,7 +6186,7 @@
       </c>
       <c r="B126" t="inlineStr"/>
       <c r="C126" t="n">
-        <v>24624.36764655067</v>
+        <v>24624.36764655068</v>
       </c>
       <c r="D126" t="inlineStr"/>
       <c r="E126" t="inlineStr"/>
@@ -6261,7 +6261,7 @@
       </c>
       <c r="B129" t="inlineStr"/>
       <c r="C129" t="n">
-        <v>5888.788401875064</v>
+        <v>5888.788401875067</v>
       </c>
       <c r="D129" t="inlineStr"/>
       <c r="E129" t="inlineStr"/>
@@ -6286,7 +6286,7 @@
       </c>
       <c r="B130" t="inlineStr"/>
       <c r="C130" t="n">
-        <v>4963.128938341389</v>
+        <v>4963.128938341388</v>
       </c>
       <c r="D130" t="inlineStr"/>
       <c r="E130" t="inlineStr"/>
@@ -6361,7 +6361,7 @@
       </c>
       <c r="B133" t="inlineStr"/>
       <c r="C133" t="n">
-        <v>3894.659362049964</v>
+        <v>3894.659362049963</v>
       </c>
       <c r="D133" t="inlineStr"/>
       <c r="E133" t="inlineStr"/>
@@ -6386,7 +6386,7 @@
       </c>
       <c r="B134" t="inlineStr"/>
       <c r="C134" t="n">
-        <v>615.1417689158059</v>
+        <v>615.1417689158056</v>
       </c>
       <c r="D134" t="inlineStr"/>
       <c r="E134" t="inlineStr"/>
@@ -6511,7 +6511,7 @@
       </c>
       <c r="B139" t="inlineStr"/>
       <c r="C139" t="n">
-        <v>3512.113637136438</v>
+        <v>3512.113637136441</v>
       </c>
       <c r="D139" t="inlineStr"/>
       <c r="E139" t="inlineStr"/>
@@ -6811,7 +6811,7 @@
       </c>
       <c r="B151" t="inlineStr"/>
       <c r="C151" t="n">
-        <v>3922.18978497749</v>
+        <v>3922.189784977491</v>
       </c>
       <c r="D151" t="inlineStr"/>
       <c r="E151" t="inlineStr"/>
@@ -6836,7 +6836,7 @@
       </c>
       <c r="B152" t="inlineStr"/>
       <c r="C152" t="n">
-        <v>6642.629150052434</v>
+        <v>6642.629150052432</v>
       </c>
       <c r="D152" t="inlineStr"/>
       <c r="E152" t="inlineStr"/>
@@ -6861,7 +6861,7 @@
       </c>
       <c r="B153" t="inlineStr"/>
       <c r="C153" t="n">
-        <v>3290.466162827486</v>
+        <v>3290.466162827488</v>
       </c>
       <c r="D153" t="inlineStr"/>
       <c r="E153" t="inlineStr"/>
@@ -6961,7 +6961,7 @@
       </c>
       <c r="B157" t="inlineStr"/>
       <c r="C157" t="n">
-        <v>2632.839746097712</v>
+        <v>2632.839746097711</v>
       </c>
       <c r="D157" t="inlineStr"/>
       <c r="E157" t="inlineStr"/>
@@ -6986,7 +6986,7 @@
       </c>
       <c r="B158" t="inlineStr"/>
       <c r="C158" t="n">
-        <v>4078.561532216292</v>
+        <v>4078.561532216293</v>
       </c>
       <c r="D158" t="inlineStr"/>
       <c r="E158" t="inlineStr"/>
@@ -7036,7 +7036,7 @@
       </c>
       <c r="B160" t="inlineStr"/>
       <c r="C160" t="n">
-        <v>4561.05535384786</v>
+        <v>4561.055353847859</v>
       </c>
       <c r="D160" t="inlineStr"/>
       <c r="E160" t="inlineStr"/>
@@ -7061,7 +7061,7 @@
       </c>
       <c r="B161" t="inlineStr"/>
       <c r="C161" t="n">
-        <v>5233.980265284601</v>
+        <v>5233.980265284602</v>
       </c>
       <c r="D161" t="inlineStr"/>
       <c r="E161" t="inlineStr"/>
@@ -7111,7 +7111,7 @@
       </c>
       <c r="B163" t="inlineStr"/>
       <c r="C163" t="n">
-        <v>7754.533509332985</v>
+        <v>7754.533509332981</v>
       </c>
       <c r="D163" t="inlineStr"/>
       <c r="E163" t="inlineStr"/>
@@ -7136,7 +7136,7 @@
       </c>
       <c r="B164" t="inlineStr"/>
       <c r="C164" t="n">
-        <v>5430.414301628933</v>
+        <v>5430.414301628931</v>
       </c>
       <c r="D164" t="inlineStr"/>
       <c r="E164" t="inlineStr"/>
@@ -7161,7 +7161,7 @@
       </c>
       <c r="B165" t="inlineStr"/>
       <c r="C165" t="n">
-        <v>6792.120605111518</v>
+        <v>6792.120605111517</v>
       </c>
       <c r="D165" t="inlineStr"/>
       <c r="E165" t="inlineStr"/>
@@ -7186,7 +7186,7 @@
       </c>
       <c r="B166" t="inlineStr"/>
       <c r="C166" t="n">
-        <v>43188.12114097897</v>
+        <v>43188.12114097898</v>
       </c>
       <c r="D166" t="inlineStr"/>
       <c r="E166" t="inlineStr"/>
@@ -7211,7 +7211,7 @@
       </c>
       <c r="B167" t="inlineStr"/>
       <c r="C167" t="n">
-        <v>37435.16717140992</v>
+        <v>37435.16717140991</v>
       </c>
       <c r="D167" t="inlineStr"/>
       <c r="E167" t="inlineStr"/>
@@ -7236,7 +7236,7 @@
       </c>
       <c r="B168" t="inlineStr"/>
       <c r="C168" t="n">
-        <v>41847.48898569804</v>
+        <v>41847.48898569801</v>
       </c>
       <c r="D168" t="inlineStr"/>
       <c r="E168" t="inlineStr"/>
@@ -7311,7 +7311,7 @@
       </c>
       <c r="B171" t="inlineStr"/>
       <c r="C171" t="n">
-        <v>68620.18341643385</v>
+        <v>68620.18341643381</v>
       </c>
       <c r="D171" t="inlineStr"/>
       <c r="E171" t="inlineStr"/>
@@ -7336,7 +7336,7 @@
       </c>
       <c r="B172" t="inlineStr"/>
       <c r="C172" t="n">
-        <v>1575.659101522368</v>
+        <v>1575.659101522366</v>
       </c>
       <c r="D172" t="inlineStr"/>
       <c r="E172" t="inlineStr"/>
@@ -7361,7 +7361,7 @@
       </c>
       <c r="B173" t="inlineStr"/>
       <c r="C173" t="n">
-        <v>11996.0493775808</v>
+        <v>11996.04937758079</v>
       </c>
       <c r="D173" t="inlineStr"/>
       <c r="E173" t="inlineStr"/>
@@ -7486,7 +7486,7 @@
       </c>
       <c r="B178" t="inlineStr"/>
       <c r="C178" t="n">
-        <v>7095.061994148668</v>
+        <v>7095.061994148669</v>
       </c>
       <c r="D178" t="inlineStr"/>
       <c r="E178" t="inlineStr"/>
@@ -7561,7 +7561,7 @@
       </c>
       <c r="B181" t="inlineStr"/>
       <c r="C181" t="n">
-        <v>6918.933286481847</v>
+        <v>6918.933286481849</v>
       </c>
       <c r="D181" t="inlineStr"/>
       <c r="E181" t="inlineStr"/>
@@ -7611,7 +7611,7 @@
       </c>
       <c r="B183" t="inlineStr"/>
       <c r="C183" t="n">
-        <v>2600.897425674296</v>
+        <v>2600.897425674295</v>
       </c>
       <c r="D183" t="inlineStr"/>
       <c r="E183" t="inlineStr"/>
@@ -7636,7 +7636,7 @@
       </c>
       <c r="B184" t="inlineStr"/>
       <c r="C184" t="n">
-        <v>3441.072825818153</v>
+        <v>3441.072825818155</v>
       </c>
       <c r="D184" t="inlineStr"/>
       <c r="E184" t="inlineStr"/>
@@ -7711,7 +7711,7 @@
       </c>
       <c r="B187" t="inlineStr"/>
       <c r="C187" t="n">
-        <v>8758.484378652372</v>
+        <v>8758.484378652371</v>
       </c>
       <c r="D187" t="inlineStr"/>
       <c r="E187" t="inlineStr"/>
@@ -7736,7 +7736,7 @@
       </c>
       <c r="B188" t="inlineStr"/>
       <c r="C188" t="n">
-        <v>11314.61351353632</v>
+        <v>11314.61351353631</v>
       </c>
       <c r="D188" t="inlineStr"/>
       <c r="E188" t="inlineStr"/>
@@ -7811,7 +7811,7 @@
       </c>
       <c r="B191" t="inlineStr"/>
       <c r="C191" t="n">
-        <v>4080.692303129855</v>
+        <v>4080.692303129856</v>
       </c>
       <c r="D191" t="inlineStr"/>
       <c r="E191" t="inlineStr"/>
@@ -7861,7 +7861,7 @@
       </c>
       <c r="B193" t="inlineStr"/>
       <c r="C193" t="n">
-        <v>22139.70318053114</v>
+        <v>22139.70318053113</v>
       </c>
       <c r="D193" t="inlineStr"/>
       <c r="E193" t="inlineStr"/>
@@ -7936,7 +7936,7 @@
       </c>
       <c r="B196" t="inlineStr"/>
       <c r="C196" t="n">
-        <v>13638.29298071653</v>
+        <v>13638.29298071655</v>
       </c>
       <c r="D196" t="inlineStr"/>
       <c r="E196" t="inlineStr"/>
@@ -7961,7 +7961,7 @@
       </c>
       <c r="B197" t="inlineStr"/>
       <c r="C197" t="n">
-        <v>57452.81282812193</v>
+        <v>57452.81282812198</v>
       </c>
       <c r="D197" t="inlineStr"/>
       <c r="E197" t="inlineStr"/>
@@ -8111,7 +8111,7 @@
       </c>
       <c r="B203" t="inlineStr"/>
       <c r="C203" t="n">
-        <v>10926.74880783117</v>
+        <v>10926.74880783116</v>
       </c>
       <c r="D203" t="inlineStr"/>
       <c r="E203" t="inlineStr"/>
@@ -8136,7 +8136,7 @@
       </c>
       <c r="B204" t="inlineStr"/>
       <c r="C204" t="n">
-        <v>8788.573208526472</v>
+        <v>8788.573208526474</v>
       </c>
       <c r="D204" t="inlineStr"/>
       <c r="E204" t="inlineStr"/>
@@ -8161,7 +8161,7 @@
       </c>
       <c r="B205" t="inlineStr"/>
       <c r="C205" t="n">
-        <v>20405.18640701603</v>
+        <v>20405.18640701604</v>
       </c>
       <c r="D205" t="inlineStr"/>
       <c r="E205" t="inlineStr"/>
@@ -8186,7 +8186,7 @@
       </c>
       <c r="B206" t="inlineStr"/>
       <c r="C206" t="n">
-        <v>25088.08673886331</v>
+        <v>25088.08673886329</v>
       </c>
       <c r="D206" t="inlineStr"/>
       <c r="E206" t="inlineStr"/>
@@ -8211,7 +8211,7 @@
       </c>
       <c r="B207" t="inlineStr"/>
       <c r="C207" t="n">
-        <v>35108.95828651691</v>
+        <v>35108.95828651692</v>
       </c>
       <c r="D207" t="inlineStr"/>
       <c r="E207" t="inlineStr"/>
@@ -8286,7 +8286,7 @@
       </c>
       <c r="B210" t="inlineStr"/>
       <c r="C210" t="n">
-        <v>7455.91402990882</v>
+        <v>7455.914029908822</v>
       </c>
       <c r="D210" t="inlineStr"/>
       <c r="E210" t="inlineStr"/>
@@ -8311,7 +8311,7 @@
       </c>
       <c r="B211" t="inlineStr"/>
       <c r="C211" t="n">
-        <v>8957.922965428061</v>
+        <v>8957.922965428063</v>
       </c>
       <c r="D211" t="inlineStr"/>
       <c r="E211" t="inlineStr"/>
@@ -8336,7 +8336,7 @@
       </c>
       <c r="B212" t="inlineStr"/>
       <c r="C212" t="n">
-        <v>5951.573241664787</v>
+        <v>5951.573241664785</v>
       </c>
       <c r="D212" t="inlineStr"/>
       <c r="E212" t="inlineStr"/>
@@ -8361,7 +8361,7 @@
       </c>
       <c r="B213" t="inlineStr"/>
       <c r="C213" t="n">
-        <v>3088.006328434872</v>
+        <v>3088.006328434873</v>
       </c>
       <c r="D213" t="inlineStr"/>
       <c r="E213" t="inlineStr"/>
@@ -8411,7 +8411,7 @@
       </c>
       <c r="B215" t="inlineStr"/>
       <c r="C215" t="n">
-        <v>9338.637999896655</v>
+        <v>9338.637999896653</v>
       </c>
       <c r="D215" t="inlineStr"/>
       <c r="E215" t="inlineStr"/>
@@ -8436,7 +8436,7 @@
       </c>
       <c r="B216" t="inlineStr"/>
       <c r="C216" t="n">
-        <v>3484.80396422284</v>
+        <v>3484.803964222841</v>
       </c>
       <c r="D216" t="inlineStr"/>
       <c r="E216" t="inlineStr"/>
@@ -8461,7 +8461,7 @@
       </c>
       <c r="B217" t="inlineStr"/>
       <c r="C217" t="n">
-        <v>4273.880541123181</v>
+        <v>4273.88054112318</v>
       </c>
       <c r="D217" t="inlineStr"/>
       <c r="E217" t="inlineStr"/>
@@ -8511,7 +8511,7 @@
       </c>
       <c r="B219" t="inlineStr"/>
       <c r="C219" t="n">
-        <v>9260.656767832284</v>
+        <v>9260.656767832281</v>
       </c>
       <c r="D219" t="inlineStr"/>
       <c r="E219" t="inlineStr"/>
@@ -8711,7 +8711,7 @@
       </c>
       <c r="B227" t="inlineStr"/>
       <c r="C227" t="n">
-        <v>7711.618706287514</v>
+        <v>7711.618706287513</v>
       </c>
       <c r="D227" t="inlineStr"/>
       <c r="E227" t="inlineStr"/>
@@ -8736,7 +8736,7 @@
       </c>
       <c r="B228" t="inlineStr"/>
       <c r="C228" t="n">
-        <v>70093.89985891023</v>
+        <v>70093.89985891021</v>
       </c>
       <c r="D228" t="inlineStr"/>
       <c r="E228" t="inlineStr"/>
@@ -8886,7 +8886,7 @@
       </c>
       <c r="B234" t="inlineStr"/>
       <c r="C234" t="n">
-        <v>11663.36482084784</v>
+        <v>11663.36482084783</v>
       </c>
       <c r="D234" t="inlineStr"/>
       <c r="E234" t="inlineStr"/>
@@ -9011,7 +9011,7 @@
       </c>
       <c r="B239" t="inlineStr"/>
       <c r="C239" t="n">
-        <v>6310.78910460972</v>
+        <v>6310.789104609717</v>
       </c>
       <c r="D239" t="inlineStr"/>
       <c r="E239" t="inlineStr"/>
@@ -9036,7 +9036,7 @@
       </c>
       <c r="B240" t="inlineStr"/>
       <c r="C240" t="n">
-        <v>38826.28812372536</v>
+        <v>38826.28812372535</v>
       </c>
       <c r="D240" t="inlineStr"/>
       <c r="E240" t="inlineStr"/>
@@ -9061,7 +9061,7 @@
       </c>
       <c r="B241" t="inlineStr"/>
       <c r="C241" t="n">
-        <v>40035.59989747014</v>
+        <v>40035.59989747013</v>
       </c>
       <c r="D241" t="inlineStr"/>
       <c r="E241" t="inlineStr"/>
@@ -9086,7 +9086,7 @@
       </c>
       <c r="B242" t="inlineStr"/>
       <c r="C242" t="n">
-        <v>27449.54586673247</v>
+        <v>27449.54586673246</v>
       </c>
       <c r="D242" t="inlineStr"/>
       <c r="E242" t="inlineStr"/>
@@ -9136,7 +9136,7 @@
       </c>
       <c r="B244" t="inlineStr"/>
       <c r="C244" t="n">
-        <v>37963.71855278253</v>
+        <v>37963.71855278257</v>
       </c>
       <c r="D244" t="inlineStr"/>
       <c r="E244" t="inlineStr"/>
@@ -9261,7 +9261,7 @@
       </c>
       <c r="B249" t="inlineStr"/>
       <c r="C249" t="n">
-        <v>27905.13789978063</v>
+        <v>27905.13789978062</v>
       </c>
       <c r="D249" t="inlineStr"/>
       <c r="E249" t="inlineStr"/>

</xml_diff>